<commit_message>
Updated budget, receipts and Frew approved block diagrams
</commit_message>
<xml_diff>
--- a/Technical/Hardware/budget.xlsx
+++ b/Technical/Hardware/budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="160" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="160" windowWidth="28680" windowHeight="17220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Guidance</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Enum</t>
   </si>
   <si>
-    <t>Total Spent</t>
-  </si>
-  <si>
     <t>Computer Totals</t>
   </si>
   <si>
@@ -112,6 +109,27 @@
   </si>
   <si>
     <t>Flight Hardware</t>
+  </si>
+  <si>
+    <t>DJI Mounting Gear</t>
+  </si>
+  <si>
+    <t>Flir Mounting Hardware</t>
+  </si>
+  <si>
+    <t>Odroids + Peripherals x 2</t>
+  </si>
+  <si>
+    <t>Final demo supplies</t>
+  </si>
+  <si>
+    <t>Cumulative Spent</t>
+  </si>
+  <si>
+    <t>Cumulative Percentage</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -154,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,12 +181,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,19 +215,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -212,14 +223,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -273,7 +286,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$22:$E$24</c:f>
+              <c:f>Sheet1!$G$28:$G$30</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -290,15 +303,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$F$24</c:f>
+              <c:f>Sheet1!$H$28:$H$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>323.39</c:v>
+                  <c:v>685.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.85</c:v>
+                  <c:v>596.67</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1461.85</c:v>
@@ -317,8 +330,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2090531096"/>
-        <c:axId val="-2084666440"/>
+        <c:axId val="2145815944"/>
+        <c:axId val="2145812920"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -331,7 +344,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$22:$E$24</c:f>
+              <c:f>Sheet1!$G$28:$G$30</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -348,18 +361,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$22:$H$24</c:f>
+              <c:f>Sheet1!$J$28:$J$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.155933333333333</c:v>
+                  <c:v>4.569933333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6216</c:v>
+                  <c:v>8.547733333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.36726666666667</c:v>
+                  <c:v>18.2934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -376,16 +389,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2085301432"/>
-        <c:axId val="-2084963096"/>
+        <c:axId val="2145800312"/>
+        <c:axId val="2145806008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090531096"/>
+        <c:axId val="2145815944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -400,7 +414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084666440"/>
+        <c:crossAx val="2145812920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -408,12 +422,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2084666440"/>
+        <c:axId val="2145812920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -447,12 +462,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090531096"/>
+        <c:crossAx val="2145815944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2084963096"/>
+        <c:axId val="2145806008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,12 +506,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085301432"/>
+        <c:crossAx val="2145800312"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2085301432"/>
+        <c:axId val="2145800312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2084963096"/>
+        <c:crossAx val="2145806008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,8 +534,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.23815939192572"/>
-          <c:y val="0.326979553305156"/>
+          <c:x val="0.137166006153204"/>
+          <c:y val="0.234336501534038"/>
           <c:w val="0.227360308285164"/>
           <c:h val="0.122607650882877"/>
         </c:manualLayout>
@@ -558,16 +573,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -911,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -923,528 +938,630 @@
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>190.49</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>B2*IF(C2=1,1,0)</f>
         <v>190.49</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>B2*IF(C2=2,1,0)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <f>B2*IF(C2=3,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>170</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D18" si="0">B3*IF(C3=1,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E18" si="1">B3*IF(C3=2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F18" si="2">B3*IF(C3=3,1,0)</f>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D22" si="0">B3*IF(C3=1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E22" si="1">B3*IF(C3=2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F22" si="2">B3*IF(C3=3,1,0)</f>
         <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>114.95</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
         <f t="shared" si="2"/>
         <v>114.95</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>49.95</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
         <f t="shared" si="2"/>
         <v>49.95</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>49.95</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
         <f t="shared" si="2"/>
         <v>49.95</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>39.9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>39.9</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>75</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7.5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>5.95</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>2</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="1"/>
         <v>5.95</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>3.95</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>2</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>3.95</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>6.95</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>2</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>6.95</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="4">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3">
         <v>800</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
         <f t="shared" si="2"/>
         <v>800</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>260</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>3</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>17</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>40</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="F17" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="5" t="s">
+      <c r="F17" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>5.5</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="F18" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="C19" t="s">
+      <c r="F18" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3">
+        <v>148</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
+      <c r="F19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.71</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>7.71</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3">
+        <v>362.1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>362.1</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="3">
+        <v>371.11</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>371.11</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="C23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1">
+        <f>SUM(D2:D22)</f>
+        <v>685.49</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SUM(E2:E22)</f>
+        <v>596.67000000000007</v>
+      </c>
+      <c r="F23" s="4">
+        <f>SUM(F2:F22)</f>
+        <v>1461.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="H27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="G28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="1">
+        <f>D23</f>
+        <v>685.49</v>
+      </c>
+      <c r="I28" s="1">
+        <f>H28</f>
+        <v>685.49</v>
+      </c>
+      <c r="J28" s="1">
+        <f>I28/$B$29*100</f>
+        <v>4.5699333333333332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="1">
+        <v>15000</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D19">
-        <f>SUM(D2:D18)</f>
-        <v>323.39</v>
-      </c>
-      <c r="E19">
-        <f>SUM(E2:E18)</f>
-        <v>69.849999999999994</v>
-      </c>
-      <c r="F19" s="3">
-        <f>SUM(F2:F18)</f>
+      <c r="H29" s="1">
+        <f>E23</f>
+        <v>596.67000000000007</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" ref="I29:I30" si="3">I28+H29</f>
+        <v>1282.1600000000001</v>
+      </c>
+      <c r="J29" s="1">
+        <f>I29/$B$29*100</f>
+        <v>8.5477333333333334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="G30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="1">
+        <f>F23</f>
         <v>1461.85</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="B21" t="s">
+      <c r="I30" s="1">
+        <f t="shared" si="3"/>
+        <v>2744.01</v>
+      </c>
+      <c r="J30" s="1">
+        <f>I30/$B$29*100</f>
+        <v>18.293400000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22">
-        <f>D19</f>
-        <v>323.39</v>
-      </c>
-      <c r="G22">
-        <f>G21+F22</f>
-        <v>323.39</v>
-      </c>
-      <c r="H22">
-        <f>G22/$A$32*100</f>
-        <v>2.1559333333333335</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23">
-        <f>E19</f>
-        <v>69.849999999999994</v>
-      </c>
-      <c r="G23">
-        <f t="shared" ref="G23:G24" si="3">G22+F23</f>
-        <v>393.24</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ref="H23:H24" si="4">G23/$A$32*100</f>
-        <v>2.6215999999999999</v>
-      </c>
-      <c r="K23">
-        <f>SUM(F22:F24)</f>
-        <v>1855.09</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B24">
+      <c r="B35" s="1">
         <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <f>F19</f>
-        <v>1461.85</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>1855.09</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>12.367266666666668</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32">
-        <v>15000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of updated shiiiiiiit
</commit_message>
<xml_diff>
--- a/Technical/Hardware/budget.xlsx
+++ b/Technical/Hardware/budget.xlsx
@@ -330,8 +330,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2145815944"/>
-        <c:axId val="2145812920"/>
+        <c:axId val="2071654520"/>
+        <c:axId val="2020657320"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -389,11 +389,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2145800312"/>
-        <c:axId val="2145806008"/>
+        <c:axId val="2099601000"/>
+        <c:axId val="2032471928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2145815944"/>
+        <c:axId val="2071654520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,7 +414,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145812920"/>
+        <c:crossAx val="2020657320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -422,7 +422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2145812920"/>
+        <c:axId val="2020657320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,12 +462,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145815944"/>
+        <c:crossAx val="2071654520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145806008"/>
+        <c:axId val="2032471928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,12 +506,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145800312"/>
+        <c:crossAx val="2099601000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2145800312"/>
+        <c:axId val="2099601000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -520,7 +520,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145806008"/>
+        <c:crossAx val="2032471928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -929,7 +929,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>